<commit_message>
added assignees for conceptual design
</commit_message>
<xml_diff>
--- a/Documentation/CapstoneTimeline.xlsx
+++ b/Documentation/CapstoneTimeline.xlsx
@@ -8,12 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\github\CapstoneRepo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAEB8C8-B63D-4BAB-A92F-ADC4115F0422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCE8B73-450E-4E4B-BA4D-41FD712FA497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7312806-6A61-4E07-9F80-D4889DE395B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="DD-Chassis" sheetId="14" r:id="rId2"/>
+    <sheet name="DD-Animal Feeding" sheetId="13" r:id="rId3"/>
+    <sheet name="DD-Location Det. and Track" sheetId="2" r:id="rId4"/>
+    <sheet name="DD-Object Detection" sheetId="3" r:id="rId5"/>
+    <sheet name="DD-Object Manipulation" sheetId="4" r:id="rId6"/>
+    <sheet name="DD-Locomotion" sheetId="5" r:id="rId7"/>
+    <sheet name="DD-Fireworks Display" sheetId="6" r:id="rId8"/>
+    <sheet name="DD-Power" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>Team Formation</t>
   </si>
@@ -131,17 +139,137 @@
     <t>Member Assignment</t>
   </si>
   <si>
-    <t>Entire Team</t>
-  </si>
-  <si>
     <t>Enitire Team</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>Assignees</t>
+  </si>
+  <si>
+    <t>Nathan Gardner</t>
+  </si>
+  <si>
+    <t>Object Manipulation</t>
+  </si>
+  <si>
+    <t>Fatima Al-heji</t>
+  </si>
+  <si>
+    <t>System Diagram</t>
+  </si>
+  <si>
+    <t>Formalated Problem Statement</t>
+  </si>
+  <si>
+    <t>Fatima Al-heji, Nathan Gardner</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Madison Kelly</t>
+  </si>
+  <si>
+    <t>Shall Statements</t>
+  </si>
+  <si>
+    <t>Ethical, Professional, and Standards Considerations</t>
+  </si>
+  <si>
+    <t>Power System</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Locomotion</t>
+  </si>
+  <si>
+    <t>Vision System</t>
+  </si>
+  <si>
+    <t>Microbot</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>System Diagram Design</t>
+  </si>
+  <si>
+    <t>Timeline and Work Breakdown</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>Mark Beech, Luke Mcgill, Nathan Gardner</t>
+  </si>
+  <si>
+    <t>Luke Mcgill</t>
+  </si>
+  <si>
+    <t>Mark Beech</t>
+  </si>
+  <si>
+    <t>LucidChart Diagrams</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Chassis</t>
+  </si>
+  <si>
+    <t>Location Determination and Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object Detection </t>
+  </si>
+  <si>
+    <t>Fireworks Display</t>
+  </si>
+  <si>
+    <t>Animal Feeding</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Mechanical Team</t>
+  </si>
+  <si>
+    <t>Mechanical Team, Fatima Al-heji, Nathan Gardner, Luke Mcgill</t>
+  </si>
+  <si>
+    <t>Madison Kelly, Mark Beech</t>
+  </si>
+  <si>
+    <t>Fatima Al-heji, Nathan Gardner, Luke Mcgill</t>
+  </si>
+  <si>
+    <t>Fatima Al-heji, Nathan Gardner, Mark Beech</t>
+  </si>
+  <si>
+    <t>DETAILED WORK BREAKDOWN</t>
+  </si>
+  <si>
+    <t>Subsystems Design</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +285,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +346,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -186,11 +361,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -206,8 +444,21 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -319,7 +570,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Main!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -357,7 +608,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Main!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -479,7 +730,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Main!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -517,7 +768,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:f>Main!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -578,7 +829,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:f>Main!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1361,8 +1612,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2151104</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>130951</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3139225" cy="1500732"/>
@@ -1379,7 +1630,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2151104" y="2728030"/>
+          <a:off x="0" y="2508391"/>
           <a:ext cx="3139225" cy="1500732"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1460,7 +1711,7 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>679250</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>61951</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1786,17 +2037,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC09B1FA-CECC-4035-B171-7CDD1AF55ECD}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" customWidth="1"/>
+    <col min="1" max="2" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.33203125" bestFit="1" customWidth="1"/>
@@ -1849,8 +2100,8 @@
         <f t="shared" ref="D3:D10" si="0">C3-B3</f>
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
+      <c r="E3" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>3</v>
@@ -1875,8 +2126,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>32</v>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>4</v>
@@ -1903,7 +2154,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>6</v>
@@ -2146,22 +2397,383 @@
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="17" t="s">
         <v>8</v>
       </c>
+      <c r="C28" s="18" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="21"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="17" t="s">
         <v>22</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="21"/>
+      <c r="C60" s="22"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="22"/>
+    </row>
+    <row r="62" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
     <sortCondition ref="B2:B15" customList="Jan,Feb,Mar,Apr,May,Jun,Jul,Aug,Sep,Oct,Nov,Dec"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B53" location="'DD-Location Det. and Track'!A1" display="Location Determination and Tracking" xr:uid="{49393598-8E01-4F0C-98F8-F3556F9E94F1}"/>
+    <hyperlink ref="B54" location="'DD-Object Detection'!A1" display="Object Detection " xr:uid="{0D9A1E34-F98F-46C4-B585-AD02F0786C59}"/>
+    <hyperlink ref="B55" location="'DD-Object Manipulation'!A1" display="Object Manipulation" xr:uid="{B61D4DCF-F653-4940-B85B-EF5BCC47C04E}"/>
+    <hyperlink ref="B56" location="'DD-Locomotion'!A1" display="Locomotion" xr:uid="{91B0B86C-16DD-45B4-BC58-57092451A29E}"/>
+    <hyperlink ref="B57" location="'DD-Fireworks Display'!A1" display="Fireworks Display" xr:uid="{945F8B7E-50D4-4ED3-AD91-EDAC8A0877A4}"/>
+    <hyperlink ref="B59" location="'DD-Power'!A1" display="Power" xr:uid="{F1ABB304-7803-4CCA-AA12-2E46549E173D}"/>
+    <hyperlink ref="B58" location="'DD-Animal Feeding'!A1" display="Animal Feeding" xr:uid="{F2F8E6E8-8B2B-4009-89DB-8B26A3DD7EFB}"/>
+    <hyperlink ref="B52" location="'DD-Chassis'!A1" display="Chassis" xr:uid="{F0F55870-F599-4F19-ADF6-BC6EBBD97A65}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA56416-B17F-4112-BC20-B5823E956BA1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA374104-B7EE-452B-9C8A-8C1A18611CDB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178B2242-6FDB-49C7-A935-72C7FD1B5A30}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930E9B9D-CE5B-422D-B24E-0ED953A1791F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7146979-0B03-48AF-A691-453D6A93343E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2115B80-C0E3-4B3F-917E-7436F3546F52}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E387DAD6-0187-40FA-BC16-0474883E7731}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7003D715-FD8D-4FAB-B335-0AEF63E3181D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Timeline/Gantt Chart Pt 2
</commit_message>
<xml_diff>
--- a/Documentation/CapstoneTimeline.xlsx
+++ b/Documentation/CapstoneTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85053780-B22A-483E-8C25-73740BCAA4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853E9A7C-4677-4CDA-9C07-A296CC13FC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7312806-6A61-4E07-9F80-D4889DE395B5}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="100">
   <si>
     <t>Team Formation</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t>Object Storage: Signoff</t>
+  </si>
+  <si>
+    <t>Fireworks Display: Detail Design and Analytical Testing</t>
+  </si>
+  <si>
+    <t>Fireworks Display: Signoff</t>
   </si>
 </sst>
 </file>
@@ -637,9 +643,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Main!$A$3:$A$29</c:f>
+              <c:f>Main!$A$3:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -692,33 +698,39 @@
                   <c:v>Locomotion Subsystem: Signoff</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Fireworks Display: Detail Design and Analytical Testing</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Fireworks Display: Signoff</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Power Subsystem: Detailed Design and Analytical Testing (LTSpice)</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>Power Subsystem: Signoff </c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>Detail Design and Planning</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Signoff</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>Ordering</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>Vision Subsystem: Programming</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>Controller Subsystem: Programming</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>Build</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>Experimentation</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>Documentation, Poster, Presentation</c:v>
                 </c:pt>
               </c:strCache>
@@ -726,10 +738,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$B$3:$B$29</c:f>
+              <c:f>Main!$B$3:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>44815</c:v>
                 </c:pt>
@@ -785,30 +797,36 @@
                   <c:v>44938</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>44945</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44938</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>44946</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>44843</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>44870</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>44870</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>44953</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>44953</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>44938</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>44986</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>45007</c:v>
                 </c:pt>
               </c:numCache>
@@ -899,9 +917,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Main!$A$3:$A$29</c:f>
+              <c:f>Main!$A$3:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>Project Proposal</c:v>
                 </c:pt>
@@ -954,33 +972,39 @@
                   <c:v>Locomotion Subsystem: Signoff</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Fireworks Display: Detail Design and Analytical Testing</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Fireworks Display: Signoff</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>Power Subsystem: Detailed Design and Analytical Testing (LTSpice)</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>Power Subsystem: Signoff </c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>Detail Design and Planning</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>Signoff</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>Ordering</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>Vision Subsystem: Programming</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>Controller Subsystem: Programming</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>Build</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>Experimentation</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>Documentation, Poster, Presentation</c:v>
                 </c:pt>
               </c:strCache>
@@ -988,10 +1012,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$D$3:$D$29</c:f>
+              <c:f>Main!$D$3:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>14</c:v>
                 </c:pt>
@@ -1047,30 +1071,36 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>109</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
@@ -1100,10 +1130,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Main!$E$3:$E$29</c:f>
+              <c:f>Main!$E$3:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1183,6 +1213,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1956,7 +1992,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>130951</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3139225" cy="1500732"/>
@@ -2054,7 +2090,7 @@
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>199293</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2380,10 +2416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC09B1FA-CECC-4035-B171-7CDD1AF55ECD}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="66" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,7 +2477,7 @@
         <v>44829</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D29" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D31" si="0">C3-B3</f>
         <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -2820,7 +2856,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B20" s="1">
         <v>44938</v>
@@ -2833,220 +2869,252 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B21" s="1">
-        <v>44946</v>
+        <v>44945</v>
       </c>
       <c r="C21" s="1">
         <v>44952</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="6">
-        <v>44948</v>
-      </c>
-      <c r="J21" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44938</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44945</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44946</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44952</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="6">
+        <v>44948</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B24" s="1">
         <f>C5</f>
         <v>44843</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C24" s="3">
         <v>44952</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H24" s="6">
         <v>44986</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B25" s="1">
         <v>44870</v>
       </c>
-      <c r="C23" s="3">
-        <f>C22</f>
+      <c r="C25" s="3">
+        <f>C24</f>
         <v>44952</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H25" s="6">
         <v>45007</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B26" s="1">
         <v>44870</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C26" s="3">
         <v>44952</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E26" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H26" s="6">
         <v>45044</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B27" s="1">
         <v>44953</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C27" s="3">
         <v>45006</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B28" s="1">
         <v>44953</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C28" s="3">
         <v>45006</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B29" s="1">
         <v>44938</v>
       </c>
-      <c r="C27" s="3">
-        <f>H22</f>
+      <c r="C29" s="3">
+        <f>H24</f>
         <v>44986</v>
       </c>
-      <c r="D27">
+      <c r="D29">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
-        <f>H22</f>
+      <c r="B30" s="3">
+        <f>H24</f>
         <v>44986</v>
       </c>
-      <c r="C28" s="3">
-        <f>H23</f>
+      <c r="C30" s="3">
+        <f>H25</f>
         <v>45007</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <f>H23</f>
+      <c r="B31" s="3">
+        <f>H25</f>
         <v>45007</v>
       </c>
-      <c r="C29" s="3">
-        <f>H24</f>
+      <c r="C31" s="3">
+        <f>H26</f>
         <v>45044</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E31" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
@@ -3061,127 +3129,119 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="9" t="s">
+    <row r="46" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="11" t="s">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="12"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>37</v>
-      </c>
+      <c r="C48" s="12"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C51" s="14" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C55" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="13"/>
-      <c r="C54" s="14"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="11" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="13"/>
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="14"/>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="15" t="s">
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C58" s="14" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>32</v>
@@ -3189,92 +3249,92 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="13"/>
-      <c r="C62" s="14"/>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="13"/>
-      <c r="C63" s="14"/>
-    </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="13"/>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="13"/>
+      <c r="C65" s="14"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C64" s="14"/>
-    </row>
-    <row r="65" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="16" t="s">
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C67" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="9" t="s">
+    <row r="68" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C69" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="11" t="s">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C68" s="14"/>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="C70" s="14"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" s="18" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" s="18" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>67</v>
@@ -3282,67 +3342,83 @@
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" s="18" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="18" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" s="18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C80" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="13"/>
-      <c r="C79" s="14"/>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="11" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="13"/>
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C80" s="14"/>
-    </row>
-    <row r="81" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="16" t="s">
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C83" s="17" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
-    <sortCondition ref="B2:B32" customList="Jan,Feb,Mar,Apr,May,Jun,Jul,Aug,Sep,Oct,Nov,Dec"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+    <sortCondition ref="B2:B34" customList="Jan,Feb,Mar,Apr,May,Jun,Jul,Aug,Sep,Oct,Nov,Dec"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B71" location="'DD-Location Det. and Track'!A1" display="Location Determination and Tracking" xr:uid="{49393598-8E01-4F0C-98F8-F3556F9E94F1}"/>
-    <hyperlink ref="B73" location="'DD-Object Detection'!A1" display="Object Detection " xr:uid="{0D9A1E34-F98F-46C4-B585-AD02F0786C59}"/>
-    <hyperlink ref="B74" location="'DD-Object Manipulation'!A1" display="Object Manipulation" xr:uid="{B61D4DCF-F653-4940-B85B-EF5BCC47C04E}"/>
-    <hyperlink ref="B75" location="'DD-Locomotion'!A1" display="Locomotion" xr:uid="{91B0B86C-16DD-45B4-BC58-57092451A29E}"/>
-    <hyperlink ref="B76" location="'DD-Fireworks Display'!A1" display="Fireworks Display" xr:uid="{945F8B7E-50D4-4ED3-AD91-EDAC8A0877A4}"/>
-    <hyperlink ref="B78" location="'DD-Power'!A1" display="Power" xr:uid="{F1ABB304-7803-4CCA-AA12-2E46549E173D}"/>
-    <hyperlink ref="B77" location="'DD-Animal Feeding'!A1" display="Animal Feeding" xr:uid="{F2F8E6E8-8B2B-4009-89DB-8B26A3DD7EFB}"/>
-    <hyperlink ref="B69" location="'DD-Chassis'!A1" display="Chassis" xr:uid="{F0F55870-F599-4F19-ADF6-BC6EBBD97A65}"/>
+    <hyperlink ref="B73" location="'DD-Location Det. and Track'!A1" display="Location Determination and Tracking" xr:uid="{49393598-8E01-4F0C-98F8-F3556F9E94F1}"/>
+    <hyperlink ref="B75" location="'DD-Object Detection'!A1" display="Object Detection " xr:uid="{0D9A1E34-F98F-46C4-B585-AD02F0786C59}"/>
+    <hyperlink ref="B76" location="'DD-Object Manipulation'!A1" display="Object Manipulation" xr:uid="{B61D4DCF-F653-4940-B85B-EF5BCC47C04E}"/>
+    <hyperlink ref="B77" location="'DD-Locomotion'!A1" display="Locomotion" xr:uid="{91B0B86C-16DD-45B4-BC58-57092451A29E}"/>
+    <hyperlink ref="B78" location="'DD-Fireworks Display'!A1" display="Fireworks Display" xr:uid="{945F8B7E-50D4-4ED3-AD91-EDAC8A0877A4}"/>
+    <hyperlink ref="B80" location="'DD-Power'!A1" display="Power" xr:uid="{F1ABB304-7803-4CCA-AA12-2E46549E173D}"/>
+    <hyperlink ref="B79" location="'DD-Animal Feeding'!A1" display="Animal Feeding" xr:uid="{F2F8E6E8-8B2B-4009-89DB-8B26A3DD7EFB}"/>
+    <hyperlink ref="B71" location="'DD-Chassis'!A1" display="Chassis" xr:uid="{F0F55870-F599-4F19-ADF6-BC6EBBD97A65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>